<commit_message>
FW file and information for the Sample Selection Forms.
</commit_message>
<xml_diff>
--- a/tables/sample-alloc.xlsx
+++ b/tables/sample-alloc.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">STRAT_PSU</t>
   </si>
@@ -23,6 +23,15 @@
     <t xml:space="preserve">strata_psu</t>
   </si>
   <si>
+    <t xml:space="preserve">strata2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reg_stat_kods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reg_stat_nosauk</t>
+  </si>
+  <si>
     <t xml:space="preserve">pop_psu</t>
   </si>
   <si>
@@ -50,19 +59,37 @@
     <t xml:space="preserve">1-1-1</t>
   </si>
   <si>
+    <t xml:space="preserve">Rīgas statistiskais reģions</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-2-2</t>
   </si>
   <si>
+    <t xml:space="preserve">Pierīgas statistiskais reģions</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-2-3</t>
   </si>
   <si>
+    <t xml:space="preserve">Vidzemes statistiskais reģions</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-2-4</t>
   </si>
   <si>
+    <t xml:space="preserve">Kurzemes statistiskais reģions</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-2-5</t>
   </si>
   <si>
+    <t xml:space="preserve">Zemgales statistiskais reģions</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-2-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latgales statistiskais reģions</t>
   </si>
   <si>
     <t xml:space="preserve">1-3-2</t>
@@ -176,20 +203,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K29" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K29"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N29" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:N29"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="STRAT_PSU"/>
     <tableColumn id="2" name="psu_cert"/>
     <tableColumn id="3" name="strata_psu"/>
-    <tableColumn id="4" name="pop_psu"/>
-    <tableColumn id="5" name="pop_du"/>
-    <tableColumn id="6" name="n_du_1"/>
-    <tableColumn id="7" name="round_base"/>
-    <tableColumn id="8" name="n_du"/>
-    <tableColumn id="9" name="f"/>
-    <tableColumn id="10" name="dw"/>
-    <tableColumn id="11" name="n_psu"/>
+    <tableColumn id="4" name="strata2019"/>
+    <tableColumn id="5" name="reg_stat_kods"/>
+    <tableColumn id="6" name="reg_stat_nosauk"/>
+    <tableColumn id="7" name="pop_psu"/>
+    <tableColumn id="8" name="pop_du"/>
+    <tableColumn id="9" name="n_du_1"/>
+    <tableColumn id="10" name="round_base"/>
+    <tableColumn id="11" name="n_du"/>
+    <tableColumn id="12" name="f"/>
+    <tableColumn id="13" name="dw"/>
+    <tableColumn id="14" name="n_psu"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -483,14 +513,17 @@
     <col min="1" max="1" width="9.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="11.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="7.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="6.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="10.71" hidden="0" customWidth="1"/>
-    <col min="8" max="8" width="4.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="11.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="11.71" hidden="0" customWidth="1"/>
-    <col min="11" max="11" width="5.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="10.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="13.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="32.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="7.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="6.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="6.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="10.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="4.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="11.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="11.71" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="5.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -527,6 +560,15 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -536,30 +578,39 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="n">
         <v>1005</v>
       </c>
-      <c r="E2" t="n">
+      <c r="H2" t="n">
         <v>239456</v>
       </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
         <v>27420</v>
       </c>
-      <c r="G2" t="n">
-        <v>15</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
+        <v>15</v>
+      </c>
+      <c r="K2" t="n">
         <v>9675</v>
       </c>
-      <c r="I2" t="n">
+      <c r="L2" t="n">
         <v>0.0404040825871976</v>
       </c>
-      <c r="J2" t="n">
+      <c r="M2" t="n">
         <v>24.7499741602067</v>
       </c>
-      <c r="K2" t="n">
+      <c r="N2" t="n">
         <v>645</v>
       </c>
     </row>
@@ -571,30 +622,39 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="n">
         <v>72</v>
       </c>
-      <c r="E3" t="n">
+      <c r="H3" t="n">
         <v>17586</v>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
         <v>27420</v>
       </c>
-      <c r="G3" t="n">
-        <v>15</v>
-      </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
+        <v>15</v>
+      </c>
+      <c r="K3" t="n">
         <v>705</v>
       </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
         <v>0.0400887069259638</v>
       </c>
-      <c r="J3" t="n">
+      <c r="M3" t="n">
         <v>24.9446808510638</v>
       </c>
-      <c r="K3" t="n">
+      <c r="N3" t="n">
         <v>47</v>
       </c>
     </row>
@@ -606,30 +666,39 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="n">
         <v>34</v>
       </c>
-      <c r="E4" t="n">
+      <c r="H4" t="n">
         <v>8004</v>
       </c>
-      <c r="F4" t="n">
+      <c r="I4" t="n">
         <v>27420</v>
       </c>
-      <c r="G4" t="n">
-        <v>15</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
+        <v>15</v>
+      </c>
+      <c r="K4" t="n">
         <v>330</v>
       </c>
-      <c r="I4" t="n">
+      <c r="L4" t="n">
         <v>0.0412293853073463</v>
       </c>
-      <c r="J4" t="n">
+      <c r="M4" t="n">
         <v>24.2545454545455</v>
       </c>
-      <c r="K4" t="n">
+      <c r="N4" t="n">
         <v>22</v>
       </c>
     </row>
@@ -641,30 +710,39 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="n">
         <v>170</v>
       </c>
-      <c r="E5" t="n">
+      <c r="H5" t="n">
         <v>38253</v>
       </c>
-      <c r="F5" t="n">
+      <c r="I5" t="n">
         <v>27420</v>
       </c>
-      <c r="G5" t="n">
-        <v>15</v>
-      </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
+        <v>15</v>
+      </c>
+      <c r="K5" t="n">
         <v>1545</v>
       </c>
-      <c r="I5" t="n">
+      <c r="L5" t="n">
         <v>0.0403889890988942</v>
       </c>
-      <c r="J5" t="n">
+      <c r="M5" t="n">
         <v>24.7592233009709</v>
       </c>
-      <c r="K5" t="n">
+      <c r="N5" t="n">
         <v>103</v>
       </c>
     </row>
@@ -676,30 +754,39 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="n">
         <v>116</v>
       </c>
-      <c r="E6" t="n">
+      <c r="H6" t="n">
         <v>27571</v>
       </c>
-      <c r="F6" t="n">
+      <c r="I6" t="n">
         <v>27420</v>
       </c>
-      <c r="G6" t="n">
-        <v>15</v>
-      </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
+        <v>15</v>
+      </c>
+      <c r="K6" t="n">
         <v>1110</v>
       </c>
-      <c r="I6" t="n">
+      <c r="L6" t="n">
         <v>0.0402596931558522</v>
       </c>
-      <c r="J6" t="n">
+      <c r="M6" t="n">
         <v>24.8387387387387</v>
       </c>
-      <c r="K6" t="n">
+      <c r="N6" t="n">
         <v>74</v>
       </c>
     </row>
@@ -711,30 +798,39 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="n">
         <v>180</v>
       </c>
-      <c r="E7" t="n">
+      <c r="H7" t="n">
         <v>41665</v>
       </c>
-      <c r="F7" t="n">
+      <c r="I7" t="n">
         <v>27420</v>
       </c>
-      <c r="G7" t="n">
-        <v>15</v>
-      </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
+        <v>15</v>
+      </c>
+      <c r="K7" t="n">
         <v>1680</v>
       </c>
-      <c r="I7" t="n">
+      <c r="L7" t="n">
         <v>0.0403216128645146</v>
       </c>
-      <c r="J7" t="n">
+      <c r="M7" t="n">
         <v>24.8005952380952</v>
       </c>
-      <c r="K7" t="n">
+      <c r="N7" t="n">
         <v>112</v>
       </c>
     </row>
@@ -746,30 +842,39 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="n">
+      <c r="G8" t="n">
         <v>174</v>
       </c>
-      <c r="E8" t="n">
+      <c r="H8" t="n">
         <v>44125</v>
       </c>
-      <c r="F8" t="n">
+      <c r="I8" t="n">
         <v>27420</v>
       </c>
-      <c r="G8" t="n">
-        <v>15</v>
-      </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
+        <v>15</v>
+      </c>
+      <c r="K8" t="n">
         <v>1785</v>
       </c>
-      <c r="I8" t="n">
+      <c r="L8" t="n">
         <v>0.0404532577903683</v>
       </c>
-      <c r="J8" t="n">
+      <c r="M8" t="n">
         <v>24.7198879551821</v>
       </c>
-      <c r="K8" t="n">
+      <c r="N8" t="n">
         <v>119</v>
       </c>
     </row>
@@ -781,30 +886,39 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="n">
         <v>87</v>
       </c>
-      <c r="E9" t="n">
+      <c r="H9" t="n">
         <v>19676</v>
       </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
         <v>27420</v>
       </c>
-      <c r="G9" t="n">
-        <v>15</v>
-      </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
+        <v>15</v>
+      </c>
+      <c r="K9" t="n">
         <v>795</v>
       </c>
-      <c r="I9" t="n">
+      <c r="L9" t="n">
         <v>0.0404045537710917</v>
       </c>
-      <c r="J9" t="n">
+      <c r="M9" t="n">
         <v>24.7496855345912</v>
       </c>
-      <c r="K9" t="n">
+      <c r="N9" t="n">
         <v>53</v>
       </c>
     </row>
@@ -816,30 +930,39 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="n">
         <v>73</v>
       </c>
-      <c r="E10" t="n">
+      <c r="H10" t="n">
         <v>16398</v>
       </c>
-      <c r="F10" t="n">
+      <c r="I10" t="n">
         <v>27420</v>
       </c>
-      <c r="G10" t="n">
-        <v>15</v>
-      </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
+        <v>15</v>
+      </c>
+      <c r="K10" t="n">
         <v>660</v>
       </c>
-      <c r="I10" t="n">
+      <c r="L10" t="n">
         <v>0.0402488108305891</v>
       </c>
-      <c r="J10" t="n">
+      <c r="M10" t="n">
         <v>24.8454545454545</v>
       </c>
-      <c r="K10" t="n">
+      <c r="N10" t="n">
         <v>44</v>
       </c>
     </row>
@@ -851,30 +974,39 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="n">
         <v>51</v>
       </c>
-      <c r="E11" t="n">
+      <c r="H11" t="n">
         <v>11766</v>
       </c>
-      <c r="F11" t="n">
+      <c r="I11" t="n">
         <v>27420</v>
       </c>
-      <c r="G11" t="n">
-        <v>15</v>
-      </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
+        <v>15</v>
+      </c>
+      <c r="K11" t="n">
         <v>480</v>
       </c>
-      <c r="I11" t="n">
+      <c r="L11" t="n">
         <v>0.0407955124936257</v>
       </c>
-      <c r="J11" t="n">
+      <c r="M11" t="n">
         <v>24.5125</v>
       </c>
-      <c r="K11" t="n">
+      <c r="N11" t="n">
         <v>32</v>
       </c>
     </row>
@@ -886,30 +1018,39 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="n">
         <v>74</v>
       </c>
-      <c r="E12" t="n">
+      <c r="H12" t="n">
         <v>16584</v>
       </c>
-      <c r="F12" t="n">
+      <c r="I12" t="n">
         <v>27420</v>
       </c>
-      <c r="G12" t="n">
-        <v>15</v>
-      </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
+        <v>15</v>
+      </c>
+      <c r="K12" t="n">
         <v>675</v>
       </c>
-      <c r="I12" t="n">
+      <c r="L12" t="n">
         <v>0.0407018813314038</v>
       </c>
-      <c r="J12" t="n">
+      <c r="M12" t="n">
         <v>24.5688888888889</v>
       </c>
-      <c r="K12" t="n">
+      <c r="N12" t="n">
         <v>45</v>
       </c>
     </row>
@@ -921,30 +1062,39 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="n">
         <v>486</v>
       </c>
-      <c r="E13" t="n">
+      <c r="H13" t="n">
         <v>69774</v>
       </c>
-      <c r="F13" t="n">
+      <c r="I13" t="n">
         <v>27420</v>
       </c>
-      <c r="G13" t="n">
-        <v>15</v>
-      </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
+        <v>15</v>
+      </c>
+      <c r="K13" t="n">
         <v>2820</v>
       </c>
-      <c r="I13" t="n">
+      <c r="L13" t="n">
         <v>0.0404162008771176</v>
       </c>
-      <c r="J13" t="n">
+      <c r="M13" t="n">
         <v>24.7425531914894</v>
       </c>
-      <c r="K13" t="n">
+      <c r="N13" t="n">
         <v>188</v>
       </c>
     </row>
@@ -956,30 +1106,39 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="n">
         <v>263</v>
       </c>
-      <c r="E14" t="n">
+      <c r="H14" t="n">
         <v>31383</v>
       </c>
-      <c r="F14" t="n">
+      <c r="I14" t="n">
         <v>27420</v>
       </c>
-      <c r="G14" t="n">
-        <v>15</v>
-      </c>
-      <c r="H14" t="n">
+      <c r="J14" t="n">
+        <v>15</v>
+      </c>
+      <c r="K14" t="n">
         <v>1260</v>
       </c>
-      <c r="I14" t="n">
+      <c r="L14" t="n">
         <v>0.0401491253226269</v>
       </c>
-      <c r="J14" t="n">
+      <c r="M14" t="n">
         <v>24.9071428571429</v>
       </c>
-      <c r="K14" t="n">
+      <c r="N14" t="n">
         <v>84</v>
       </c>
     </row>
@@ -991,30 +1150,39 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D15" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="n">
         <v>219</v>
       </c>
-      <c r="E15" t="n">
+      <c r="H15" t="n">
         <v>26187</v>
       </c>
-      <c r="F15" t="n">
+      <c r="I15" t="n">
         <v>27420</v>
       </c>
-      <c r="G15" t="n">
-        <v>15</v>
-      </c>
-      <c r="H15" t="n">
+      <c r="J15" t="n">
+        <v>15</v>
+      </c>
+      <c r="K15" t="n">
         <v>1065</v>
       </c>
-      <c r="I15" t="n">
+      <c r="L15" t="n">
         <v>0.0406690342536373</v>
       </c>
-      <c r="J15" t="n">
+      <c r="M15" t="n">
         <v>24.5887323943662</v>
       </c>
-      <c r="K15" t="n">
+      <c r="N15" t="n">
         <v>71</v>
       </c>
     </row>
@@ -1026,30 +1194,39 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="n">
         <v>294</v>
       </c>
-      <c r="E16" t="n">
+      <c r="H16" t="n">
         <v>37017</v>
       </c>
-      <c r="F16" t="n">
+      <c r="I16" t="n">
         <v>27420</v>
       </c>
-      <c r="G16" t="n">
-        <v>15</v>
-      </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
+        <v>15</v>
+      </c>
+      <c r="K16" t="n">
         <v>1500</v>
       </c>
-      <c r="I16" t="n">
+      <c r="L16" t="n">
         <v>0.0405219223599968</v>
       </c>
-      <c r="J16" t="n">
+      <c r="M16" t="n">
         <v>24.678</v>
       </c>
-      <c r="K16" t="n">
+      <c r="N16" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1061,30 +1238,39 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D17" t="n">
+        <v>4</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" t="n">
         <v>291</v>
       </c>
-      <c r="E17" t="n">
+      <c r="H17" t="n">
         <v>33011</v>
       </c>
-      <c r="F17" t="n">
+      <c r="I17" t="n">
         <v>27420</v>
       </c>
-      <c r="G17" t="n">
-        <v>15</v>
-      </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
+        <v>15</v>
+      </c>
+      <c r="K17" t="n">
         <v>1335</v>
       </c>
-      <c r="I17" t="n">
+      <c r="L17" t="n">
         <v>0.0404410650995123</v>
       </c>
-      <c r="J17" t="n">
+      <c r="M17" t="n">
         <v>24.72734082397</v>
       </c>
-      <c r="K17" t="n">
+      <c r="N17" t="n">
         <v>89</v>
       </c>
     </row>
@@ -1096,30 +1282,39 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
       </c>
       <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
         <v>382</v>
       </c>
-      <c r="F18" t="n">
+      <c r="I18" t="n">
         <v>210</v>
       </c>
-      <c r="G18" t="n">
-        <v>3</v>
-      </c>
-      <c r="H18" t="n">
-        <v>15</v>
-      </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
+        <v>3</v>
+      </c>
+      <c r="K18" t="n">
+        <v>15</v>
+      </c>
+      <c r="L18" t="n">
         <v>0.0392670157068063</v>
       </c>
-      <c r="J18" t="n">
+      <c r="M18" t="n">
         <v>25.4666666666667</v>
       </c>
-      <c r="K18" t="n">
+      <c r="N18" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1131,30 +1326,39 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
       </c>
       <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
         <v>435</v>
       </c>
-      <c r="F19" t="n">
+      <c r="I19" t="n">
         <v>210</v>
       </c>
-      <c r="G19" t="n">
-        <v>3</v>
-      </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
+        <v>3</v>
+      </c>
+      <c r="K19" t="n">
         <v>18</v>
       </c>
-      <c r="I19" t="n">
+      <c r="L19" t="n">
         <v>0.0413793103448276</v>
       </c>
-      <c r="J19" t="n">
+      <c r="M19" t="n">
         <v>24.1666666666667</v>
       </c>
-      <c r="K19" t="n">
+      <c r="N19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1166,30 +1370,39 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D20" t="n">
         <v>1</v>
       </c>
       <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
         <v>431</v>
       </c>
-      <c r="F20" t="n">
+      <c r="I20" t="n">
         <v>210</v>
       </c>
-      <c r="G20" t="n">
-        <v>3</v>
-      </c>
-      <c r="H20" t="n">
+      <c r="J20" t="n">
+        <v>3</v>
+      </c>
+      <c r="K20" t="n">
         <v>18</v>
       </c>
-      <c r="I20" t="n">
+      <c r="L20" t="n">
         <v>0.0417633410672854</v>
       </c>
-      <c r="J20" t="n">
+      <c r="M20" t="n">
         <v>23.9444444444444</v>
       </c>
-      <c r="K20" t="n">
+      <c r="N20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1201,30 +1414,39 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D21" t="n">
         <v>1</v>
       </c>
       <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
         <v>402</v>
       </c>
-      <c r="F21" t="n">
+      <c r="I21" t="n">
         <v>210</v>
       </c>
-      <c r="G21" t="n">
-        <v>3</v>
-      </c>
-      <c r="H21" t="n">
+      <c r="J21" t="n">
+        <v>3</v>
+      </c>
+      <c r="K21" t="n">
         <v>18</v>
       </c>
-      <c r="I21" t="n">
+      <c r="L21" t="n">
         <v>0.0447761194029851</v>
       </c>
-      <c r="J21" t="n">
+      <c r="M21" t="n">
         <v>22.3333333333333</v>
       </c>
-      <c r="K21" t="n">
+      <c r="N21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1236,30 +1458,39 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
       </c>
       <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
         <v>395</v>
       </c>
-      <c r="F22" t="n">
+      <c r="I22" t="n">
         <v>210</v>
       </c>
-      <c r="G22" t="n">
-        <v>3</v>
-      </c>
-      <c r="H22" t="n">
-        <v>15</v>
-      </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
+        <v>3</v>
+      </c>
+      <c r="K22" t="n">
+        <v>15</v>
+      </c>
+      <c r="L22" t="n">
         <v>0.0379746835443038</v>
       </c>
-      <c r="J22" t="n">
+      <c r="M22" t="n">
         <v>26.3333333333333</v>
       </c>
-      <c r="K22" t="n">
+      <c r="N22" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1271,30 +1502,39 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
       </c>
       <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
         <v>402</v>
       </c>
-      <c r="F23" t="n">
+      <c r="I23" t="n">
         <v>210</v>
       </c>
-      <c r="G23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H23" t="n">
+      <c r="J23" t="n">
+        <v>3</v>
+      </c>
+      <c r="K23" t="n">
         <v>18</v>
       </c>
-      <c r="I23" t="n">
+      <c r="L23" t="n">
         <v>0.0447761194029851</v>
       </c>
-      <c r="J23" t="n">
+      <c r="M23" t="n">
         <v>22.3333333333333</v>
       </c>
-      <c r="K23" t="n">
+      <c r="N23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1306,30 +1546,39 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D24" t="n">
         <v>1</v>
       </c>
       <c r="E24" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
         <v>489</v>
       </c>
-      <c r="F24" t="n">
+      <c r="I24" t="n">
         <v>210</v>
       </c>
-      <c r="G24" t="n">
-        <v>3</v>
-      </c>
-      <c r="H24" t="n">
+      <c r="J24" t="n">
+        <v>3</v>
+      </c>
+      <c r="K24" t="n">
         <v>21</v>
       </c>
-      <c r="I24" t="n">
+      <c r="L24" t="n">
         <v>0.0429447852760736</v>
       </c>
-      <c r="J24" t="n">
+      <c r="M24" t="n">
         <v>23.2857142857143</v>
       </c>
-      <c r="K24" t="n">
+      <c r="N24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1341,30 +1590,39 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D25" t="n">
         <v>1</v>
       </c>
       <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
         <v>406</v>
       </c>
-      <c r="F25" t="n">
+      <c r="I25" t="n">
         <v>210</v>
       </c>
-      <c r="G25" t="n">
-        <v>3</v>
-      </c>
-      <c r="H25" t="n">
+      <c r="J25" t="n">
+        <v>3</v>
+      </c>
+      <c r="K25" t="n">
         <v>18</v>
       </c>
-      <c r="I25" t="n">
+      <c r="L25" t="n">
         <v>0.0443349753694581</v>
       </c>
-      <c r="J25" t="n">
+      <c r="M25" t="n">
         <v>22.5555555555556</v>
       </c>
-      <c r="K25" t="n">
+      <c r="N25" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1376,30 +1634,39 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>
       </c>
       <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
         <v>381</v>
       </c>
-      <c r="F26" t="n">
+      <c r="I26" t="n">
         <v>210</v>
       </c>
-      <c r="G26" t="n">
-        <v>3</v>
-      </c>
-      <c r="H26" t="n">
-        <v>15</v>
-      </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
+        <v>3</v>
+      </c>
+      <c r="K26" t="n">
+        <v>15</v>
+      </c>
+      <c r="L26" t="n">
         <v>0.0393700787401575</v>
       </c>
-      <c r="J26" t="n">
+      <c r="M26" t="n">
         <v>25.4</v>
       </c>
-      <c r="K26" t="n">
+      <c r="N26" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1411,30 +1678,39 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
       </c>
       <c r="E27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" t="n">
         <v>455</v>
       </c>
-      <c r="F27" t="n">
+      <c r="I27" t="n">
         <v>210</v>
       </c>
-      <c r="G27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H27" t="n">
+      <c r="J27" t="n">
+        <v>3</v>
+      </c>
+      <c r="K27" t="n">
         <v>18</v>
       </c>
-      <c r="I27" t="n">
+      <c r="L27" t="n">
         <v>0.0395604395604396</v>
       </c>
-      <c r="J27" t="n">
+      <c r="M27" t="n">
         <v>25.2777777777778</v>
       </c>
-      <c r="K27" t="n">
+      <c r="N27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1446,30 +1722,39 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D28" t="n">
         <v>1</v>
       </c>
       <c r="E28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" t="n">
         <v>396</v>
       </c>
-      <c r="F28" t="n">
+      <c r="I28" t="n">
         <v>210</v>
       </c>
-      <c r="G28" t="n">
-        <v>3</v>
-      </c>
-      <c r="H28" t="n">
-        <v>15</v>
-      </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
+        <v>3</v>
+      </c>
+      <c r="K28" t="n">
+        <v>15</v>
+      </c>
+      <c r="L28" t="n">
         <v>0.0378787878787879</v>
       </c>
-      <c r="J28" t="n">
+      <c r="M28" t="n">
         <v>26.4</v>
       </c>
-      <c r="K28" t="n">
+      <c r="N28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1481,30 +1766,39 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E29" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" t="n">
         <v>545</v>
       </c>
-      <c r="F29" t="n">
+      <c r="I29" t="n">
         <v>210</v>
       </c>
-      <c r="G29" t="n">
-        <v>3</v>
-      </c>
-      <c r="H29" t="n">
+      <c r="J29" t="n">
+        <v>3</v>
+      </c>
+      <c r="K29" t="n">
         <v>21</v>
       </c>
-      <c r="I29" t="n">
+      <c r="L29" t="n">
         <v>0.0385321100917431</v>
       </c>
-      <c r="J29" t="n">
+      <c r="M29" t="n">
         <v>25.952380952381</v>
       </c>
-      <c r="K29" t="n">
+      <c r="N29" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>